<commit_message>
[main:feat] adding datatables to dashboard and user dashboard
</commit_message>
<xml_diff>
--- a/storage/kumuhR0.xlsx
+++ b/storage/kumuhR0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riqqi\OneDrive\Desktop\motorkawanku-be\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8044C510-A912-4E6D-8D84-8698C06140C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2C9C5E-AD69-418C-8ED9-2EF9A08C772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{D43C3B05-5343-47FE-994A-9761FB850A74}"/>
   </bookViews>
@@ -1748,6 +1748,141 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="61" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="4" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1760,18 +1895,18 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1780,141 +1915,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="4" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2492,7 +2492,7 @@
       <pane xSplit="6" ySplit="13" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,14 +2513,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
+      <c r="A1" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2530,8 +2530,8 @@
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
+      <c r="A2" s="159"/>
+      <c r="B2" s="159"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="10" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
-      <c r="B10" s="168">
+      <c r="B10" s="113">
         <f>SUMIFS(kawasan[id],kawasan[rt-rw],$B$8)</f>
         <v>0</v>
       </c>
@@ -2712,52 +2712,52 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="115" t="s">
+      <c r="A11" s="160" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="137" t="s">
+      <c r="D11" s="164"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="165"/>
+      <c r="G11" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="138"/>
-      <c r="I11" s="139"/>
-      <c r="J11" s="124" t="s">
+      <c r="H11" s="156"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="125"/>
-      <c r="L11" s="125"/>
-      <c r="M11" s="126"/>
+      <c r="K11" s="145"/>
+      <c r="L11" s="145"/>
+      <c r="M11" s="146"/>
       <c r="N11" s="54"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="130" t="s">
+      <c r="A12" s="161"/>
+      <c r="B12" s="162"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="168"/>
+      <c r="G12" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="131"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="127"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="128"/>
-      <c r="M12" s="129"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="148"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="149"/>
       <c r="N12" s="54"/>
     </row>
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
-      <c r="B13" s="118"/>
+      <c r="A13" s="161"/>
+      <c r="B13" s="162"/>
       <c r="C13" s="16" t="s">
         <v>19</v>
       </c>
@@ -2794,7 +2794,7 @@
       <c r="N13" s="54"/>
     </row>
     <row r="14" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="133" t="s">
+      <c r="A14" s="132" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="60" t="s">
@@ -2843,7 +2843,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="133"/>
+      <c r="A15" s="132"/>
       <c r="B15" s="60" t="s">
         <v>28</v>
       </c>
@@ -2890,7 +2890,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="134"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="67" t="s">
         <v>29</v>
       </c>
@@ -2937,12 +2937,12 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="141"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
       <c r="E17" s="48" t="e">
         <f>IF(SUM(F14:F16)&gt;0,(SUMIF(F14:F16,"&gt;0",E14:E16)/3),0)</f>
         <v>#DIV/0!</v>
@@ -2961,7 +2961,7 @@
       <c r="N17" s="54"/>
     </row>
     <row r="18" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="154" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="72" t="s">
@@ -3010,7 +3010,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136"/>
+      <c r="A19" s="133"/>
       <c r="B19" s="60" t="s">
         <v>34</v>
       </c>
@@ -3057,12 +3057,12 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="140" t="s">
+      <c r="A20" s="128" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="129"/>
       <c r="E20" s="48" t="e">
         <f>IF(SUM(F18:F19)&gt;0,(SUMIF(F18:F19,"&gt;0",E18:E19)/2),0)</f>
         <v>#DIV/0!</v>
@@ -3081,7 +3081,7 @@
       <c r="N20" s="54"/>
     </row>
     <row r="21" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="133" t="s">
+      <c r="A21" s="132" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="60" t="s">
@@ -3130,7 +3130,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="133"/>
+      <c r="A22" s="132"/>
       <c r="B22" s="60" t="s">
         <v>38</v>
       </c>
@@ -3177,12 +3177,12 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="140" t="s">
+      <c r="A23" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="141"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
       <c r="E23" s="48" t="e">
         <f>IF(SUM(F21:F22)&gt;0,(SUMIF(F21:F22,"&gt;0",E21:E22)/2),0)</f>
         <v>#DIV/0!</v>
@@ -3201,7 +3201,7 @@
       <c r="N23" s="54"/>
     </row>
     <row r="24" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="136" t="s">
+      <c r="A24" s="133" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="77" t="s">
@@ -3250,7 +3250,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="136"/>
+      <c r="A25" s="133"/>
       <c r="B25" s="60" t="s">
         <v>42</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="136"/>
+      <c r="A26" s="133"/>
       <c r="B26" s="77" t="s">
         <v>43</v>
       </c>
@@ -3344,12 +3344,12 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="152" t="s">
+      <c r="A27" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="153"/>
-      <c r="C27" s="153"/>
-      <c r="D27" s="153"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="131"/>
+      <c r="D27" s="131"/>
       <c r="E27" s="48" t="e">
         <f>IF(SUM(F24:F26)&gt;0,(SUMIF(F24:F26,"&gt;0",E24:E26)/3),0)</f>
         <v>#DIV/0!</v>
@@ -3368,7 +3368,7 @@
       <c r="N27" s="54"/>
     </row>
     <row r="28" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="133" t="s">
+      <c r="A28" s="132" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="60" t="s">
@@ -3417,7 +3417,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="133"/>
+      <c r="A29" s="132"/>
       <c r="B29" s="60" t="s">
         <v>47</v>
       </c>
@@ -3464,12 +3464,12 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="152" t="s">
+      <c r="A30" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="131"/>
+      <c r="D30" s="131"/>
       <c r="E30" s="48" t="e">
         <f>IF(SUM(F28:F29)&gt;0,(SUMIF(F28:F29,"&gt;0",E28:E29)/2),0)</f>
         <v>#DIV/0!</v>
@@ -3488,7 +3488,7 @@
       <c r="N30" s="54"/>
     </row>
     <row r="31" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="136" t="s">
+      <c r="A31" s="133" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="60" t="s">
@@ -3537,7 +3537,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="136"/>
+      <c r="A32" s="133"/>
       <c r="B32" s="60" t="s">
         <v>51</v>
       </c>
@@ -3584,12 +3584,12 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="152" t="s">
+      <c r="A33" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="153"/>
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="131"/>
       <c r="E33" s="48" t="e">
         <f>IF(SUM(F31:F32)&gt;0,(SUMIF(F31:F32,"&gt;0",E31:E32)/2),0)</f>
         <v>#DIV/0!</v>
@@ -3608,7 +3608,7 @@
       <c r="N33" s="54"/>
     </row>
     <row r="34" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="132" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="82" t="s">
@@ -3657,7 +3657,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="133"/>
+      <c r="A35" s="132"/>
       <c r="B35" s="82" t="s">
         <v>55</v>
       </c>
@@ -3704,12 +3704,12 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="152" t="s">
+      <c r="A36" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="153"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
       <c r="E36" s="48" t="e">
         <f>IF(SUM(F34:F35)&gt;0,(SUMIF(F34:F35,"&gt;0",E34:E35)/2),0)</f>
         <v>#DIV/0!</v>
@@ -3733,11 +3733,11 @@
         <v>57</v>
       </c>
       <c r="C37" s="63"/>
-      <c r="D37" s="142" t="s">
+      <c r="D37" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="143"/>
-      <c r="F37" s="146" t="e">
+      <c r="E37" s="135"/>
+      <c r="F37" s="138" t="e">
         <f>SUM(F14:F16,F18:F19,F21:F22,F24:F25,F26,F28:F29,F31:F32,F34:F35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3745,11 +3745,11 @@
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
-      <c r="K37" s="148" t="s">
+      <c r="K37" s="140" t="s">
         <v>58</v>
       </c>
-      <c r="L37" s="149"/>
-      <c r="M37" s="154" t="e">
+      <c r="L37" s="141"/>
+      <c r="M37" s="114" t="e">
         <f>SUM(M14:M16,M18:M19,M21:M22,M24:M25,M26,M28:M29,M31:M32,M34:M35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3761,16 +3761,16 @@
         <v>59</v>
       </c>
       <c r="C38" s="63"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="147"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="139"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
       <c r="J38" s="23"/>
-      <c r="K38" s="150"/>
-      <c r="L38" s="151"/>
-      <c r="M38" s="155"/>
+      <c r="K38" s="142"/>
+      <c r="L38" s="143"/>
+      <c r="M38" s="115"/>
       <c r="N38" s="54"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3779,11 +3779,11 @@
         <v>60</v>
       </c>
       <c r="C39" s="63"/>
-      <c r="D39" s="156" t="s">
+      <c r="D39" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="157"/>
-      <c r="F39" s="160" t="e">
+      <c r="E39" s="117"/>
+      <c r="F39" s="120" t="e">
         <f>IF(F37="N/A","TIDAK KUMUH",IF(F37&gt;=60,"KUMUH BERAT",IF(AND(F37&lt;=59,F37&gt;=38),"KUMUH SEDANG",IF(AND(F37&lt;=37,F37&gt;=16),"KUMUH RINGAN","TIDAK KUMUH"))))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3791,11 +3791,11 @@
       <c r="H39" s="53"/>
       <c r="I39" s="53"/>
       <c r="J39" s="53"/>
-      <c r="K39" s="162" t="s">
+      <c r="K39" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="L39" s="163"/>
-      <c r="M39" s="166" t="e">
+      <c r="L39" s="123"/>
+      <c r="M39" s="126" t="e">
         <f>IF(M37="N/A","TIDAK KUMUH",IF(M37&gt;=60,"KUMUH BERAT",IF(AND(M37&lt;=59,M37&gt;=38),"KUMUH SEDANG",IF(AND(M37&lt;=37,M37&gt;=16),"KUMUH RINGAN","TIDAK KUMUH"))))</f>
         <v>#DIV/0!</v>
       </c>
@@ -3807,16 +3807,16 @@
         <v>62</v>
       </c>
       <c r="C40" s="63"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="159"/>
-      <c r="F40" s="161"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="121"/>
       <c r="G40" s="53"/>
       <c r="H40" s="53"/>
       <c r="I40" s="53"/>
       <c r="J40" s="53"/>
-      <c r="K40" s="164"/>
-      <c r="L40" s="165"/>
-      <c r="M40" s="167"/>
+      <c r="K40" s="124"/>
+      <c r="L40" s="125"/>
+      <c r="M40" s="127"/>
       <c r="N40" s="54"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3874,23 +3874,11 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="D39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="K39:L40"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="K37:L38"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:F12"/>
     <mergeCell ref="J11:M12"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="A14:A16"/>
@@ -3899,11 +3887,23 @@
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:F12"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="K37:L38"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="K39:L40"/>
+    <mergeCell ref="M39:M40"/>
   </mergeCells>
   <conditionalFormatting sqref="F39:F40">
     <cfRule type="expression" dxfId="17" priority="22">

</xml_diff>